<commit_message>
Update CV for DCN lab of networking and cloud computing
</commit_message>
<xml_diff>
--- a/_self/_lab_informations/labInformation.xlsx
+++ b/_self/_lab_informations/labInformation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trieu/Documents/gitWork/_docs_sources/_self/_lab_informations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC252BB-1B9D-9646-8424-3CB26F9894FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41FF6A2-4249-FE44-B5CC-54671441BF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19340" xr2:uid="{2025ECE5-ACCE-EB42-A8EF-DFF6BEA1AEC9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" xr2:uid="{2025ECE5-ACCE-EB42-A8EF-DFF6BEA1AEC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Lab_Informations" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>No</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>http://dcnlab.ssu.ac.kr/topics/</t>
-  </si>
-  <si>
-    <t>SOONGSIL UNIVERSITY</t>
   </si>
   <si>
     <t>https://www.facebook.com/groups/hbgshq</t>
@@ -168,6 +165,81 @@
 Distributed Tracing Environment Automation System
 Proxy &amp; Instrumentation Integrated Sidecar
 AI-based Infra Management</t>
+  </si>
+  <si>
+    <t>[Thông tin Học Bổng Combine/PhD tại trường Pusan National University, học kỳ mùa Thu 2023]
+Xin chào mọi người! Do chưa tìm được sinh viên phù hợp nên mình xin phép đăng lại thông tin học bổng như sau:
+Hiện tại lab của mình đang cần tuyển 01 sinh viên Combine/PhD vào kỳ mùa Thu 2023.
+Dưới đây là thông tin về giáo sư cũng như hướng nghiên cứu trong lab:
+Professor Choi Joon Young (Department of Electrical and Electronics Engineering) [https://ecsl.pusan.ac.kr/esleng/30458/subview.do], Embedded Control System Lab., Pusan ​​National University.
+Main research topic: Embedded Control System, Servo Motor Control System, Embedded Linux, Industrial Communication Network, IoT
+Requirements:
+English requirements: TOEIC &gt;=700 or IELTS &gt;=5.5 or TOELF PBT 550, iBT 80.
+Graduated from universities majoring in Electrical and Electronics, Electronics and Telecommunication, Computer Science, Computer Engineering, ... including Hanoi University of Science and Technology, Vietnam National University Hanoi, National University of HCM City, ... interested in control system or embedded system.
+GPA: &gt; 3.0/4.0
+Support from professor: for combined program, starts from 1,300,000 won/month, 200,000 won/month increased each year until the fourth year (including tuition fee), for PhD., starts from 1,500,000 won/month (including tuition fee)
+Experiences in one of the followings will have advantages:
+Advanced experiences in C/C++ programming.
+Experienced in microprocessor/microcontroller programming with Texas Instrument devices with Code Compose Studio.
+Experienced in working with Linux/Unix (kernel rebuild).
+Have knowledge of data transmission techniques (UART/SPI/I2C/Ethernet/EtherCAT...).
+Have knowledge of different kinds of electric motors.
+Bạn nào có quan tâm xin gửi email gồm CV, bảng điểm, chứng chỉ tiếng Anh cho mình qua email ductran.cse@gmail.com hoặc liên hệ trực tiếp với giáo sư!
+Cảm ơn mọi người đã đọc!</t>
+  </si>
+  <si>
+    <t>https://ecsl.pusan.ac.kr/esleng/29072/subview.do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.facebook.com/groups/hbgshq/permalink/6239860969409867/ </t>
+  </si>
+  <si>
+    <t>Pusan National University (ECSL - Embedded Control System Lab)</t>
+  </si>
+  <si>
+    <t>SOONGSIL UNIVERSITY - DCN Lab</t>
+  </si>
+  <si>
+    <t>Sejong University - IVCLab</t>
+  </si>
+  <si>
+    <t>Specific Field of Research:
+· Image Processing and Computer Vision in Video Compression techniques for virtual reality applications, such as 6 DoF immersive video or 360-Degree Video.
+· Image Processing and Computer Vision in some real-world projects, such as Autonomous Unmanned Vehicle or AI Camera.
+. Reconstruct 3D objects or some tasks related to the factory.</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/view/ivcl?fbclid=IwAR2Rf2G3Y2tg7QmbJJP82ZGA7YLgE1LlVglYpVRD5lm8vCAor021Y2mXflI</t>
+  </si>
+  <si>
+    <t>[IVCLab - M.S./Joint M.S.-Ph.D positions - Intelligent Mechatronics Engineering, Sejong University]
+Image Processing/ Computer Vision/ Video Compression
+Xin chào mọi người, lại là mình cùng thông tin tuyển sinh M.S và Combined hoặc có thể PhD cho lab.
+Specific Field of Research:
+· Image Processing and Computer Vision in Video Compression techniques for virtual reality applications, such as 6 DoF immersive video or 360-Degree Video.
+· Image Processing and Computer Vision in some real-world projects, such as Autonomous Unmanned Vehicle or AI Camera.
+. Reconstruct 3D objects or some tasks related to the factory.
+Eligibility Requirements:
+· B.S. Degree Holders in Related Field
+· English: Proficiency in Speaking and Writing
+Financial Aid:
+· Full Scholarship
+· About 1,300,000+ Korean Won Per Month on Average + incentive depending on the project.
+Lab Equipment:
+· The personal computers and servers with good configuration.
+-------------
+Giáo chăm sinh viên kỹ, thoải mái trong tiền bạc và giờ giấc. Trừ chuyện giáo không hỗ trợ con dấu để làm VISA (giáo giải thích là giáo quan ngại về rò rỷ thông tin cá nhân) thì mọi thứ từ trang thiết bị, lương, bonus, hỗ trợ bữa ăn tối mỗi ngày, đến hỗ trợ sửa viết báo đều rất oke. Lương ở trên là min, có thể tăng theo thái độ và năng lực.
+Về thiết bị của Lab thì đang có tầm 6 con server với tổng 12 GPU A100 80Gb và 6 A100 40 Gb thêm nhiều con TITAN 24 Gb. Nếu thêm người thì giáo lại tiếp tục mua server mới. Máy cá nhân thì RTX 3090 TI. Dự án của giáo đang có xu hướng chuyển dịch từ dần sang computer vision kết hợp với automation nhiều hơn là thuần xử lý ảnh và video.
+Trên đây là những dòng tâm sự mong tuyển được sinh viên chớ em cũng mệt về dụ VISA này lắm. Tuy nhiên, như em đã trình bày, trừ dụ VISA ra thì giáo rất tốt tính và công bằng. Qua đây em cũng hy vọng nhận được một số ý kiến về giải pháp từ những anh chị và các bạn có kinh nghiệm trong vấn đề này.
+Mọi người quan tâm hay có thắc mắc có thể liên hệ trực tiếp với em qua facebook cá nhân hoặc email: vanthe.le96@gmail.com.
+Thông tin về lab và các dự án lab đang tham gia mọi người có thể tham khảo tại: https://sites.google.com/view/ivcl
+Cảm ơn mọi người đã quan tâm. Thân ái và quyết thắng cùng bản tin tuyển sinh tự chứng minh tài chính.</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/groups/hbgshq/permalink/6243290112400286/</t>
+  </si>
+  <si>
+    <t>Seoul</t>
   </si>
 </sst>
 </file>
@@ -219,37 +291,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -566,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E3FAE0-FEA8-534C-A98C-B63B3E9EAC4A}">
-  <dimension ref="B3:H15"/>
+  <dimension ref="B3:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,182 +658,253 @@
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="1" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="75.1640625" style="1" customWidth="1"/>
     <col min="6" max="7" width="37.33203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="2:8" ht="264" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="10">
+        <v>2</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="F13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="264" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="2:8" ht="264" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="2:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:8" ht="264" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="2">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="264" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="2:8" ht="264" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="H4:H12"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="G4:G12"/>
     <mergeCell ref="C4:C12"/>
     <mergeCell ref="B4:B12"/>
     <mergeCell ref="E4:E12"/>
     <mergeCell ref="F4:F12"/>
     <mergeCell ref="F13:F15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" xr:uid="{F8EA4801-D202-AD44-8583-E80F5D3085C5}"/>
-    <hyperlink ref="F13" r:id="rId2" xr:uid="{2CD9648F-25F4-6D4E-B673-35983BF3ED2B}"/>
-    <hyperlink ref="G13" r:id="rId3" xr:uid="{AF98EEA4-9FD1-C344-9B16-E5D175B3CD59}"/>
+    <hyperlink ref="G13" r:id="rId2" xr:uid="{AF98EEA4-9FD1-C344-9B16-E5D175B3CD59}"/>
+    <hyperlink ref="F13" r:id="rId3" xr:uid="{2CD9648F-25F4-6D4E-B673-35983BF3ED2B}"/>
+    <hyperlink ref="F16" r:id="rId4" xr:uid="{81B9ACA6-538E-2F45-9F5F-F17705F0F145}"/>
+    <hyperlink ref="G16" r:id="rId5" xr:uid="{0CB32681-B7CB-0E47-8CA5-BF7E8D3DB0D6}"/>
+    <hyperlink ref="F17" r:id="rId6" xr:uid="{52DD9A9E-469C-C947-BAA4-F83311882240}"/>
+    <hyperlink ref="G17" r:id="rId7" xr:uid="{DEC203D3-3B05-DD4B-99B5-064ABE48C12E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove DS_Store and adding new files for edge cloud lab
</commit_message>
<xml_diff>
--- a/_self/_lab_informations/labInformation.xlsx
+++ b/_self/_lab_informations/labInformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trieu/Documents/gitWork/_docs_sources/_self/_lab_informations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41FF6A2-4249-FE44-B5CC-54671441BF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBE7C6A-BDA9-624D-B9C1-55D688744443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19300" xr2:uid="{2025ECE5-ACCE-EB42-A8EF-DFF6BEA1AEC9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>No</t>
   </si>
@@ -240,6 +240,48 @@
   </si>
   <si>
     <t>Seoul</t>
+  </si>
+  <si>
+    <t>Chungbuk University - NCLab</t>
+  </si>
+  <si>
+    <t>Chào mọi người,
+Lab mình (NCLab- Chungbuk National University) đang tuyển thêm sinh viên PhD, Combined và Master cho kì thu tháng 9/2023.
+Thông tin như sau:
+1/ Yêu cầu: có kiến thức nền tảng về 1 trong các mảng như Edge Computing, Container Orchestration và Kubernetes, Machine Learning, Federated Learning và Edge AI. Tiếng anh yêu cầu có thể giao tiếp được với giáo sư trong quá trình phỏng vấn.
+2/ Quyền lợi (Học phí~3,000,000 won/ 1 kì =&gt; tương ứng mỗi tháng 500,000 won):
+👉Master: 1,400,000 won/ tháng
+👉Phd:
++ 1,800,000 won/ tháng (2 năm đầu)
++ 2,000,000 won/ tháng (1 năm cuối)
+👉Combined:
++ 1,600,000 won/ tháng (2 năm đầu)
++ 2,000,000 won/ tháng (3 năm cuối)
+Ngoài ra cuối mỗi học kì giáo sư đều thưởng riêng nếu có performance tốt và publish paper.
+3/ Thông tin khác:
++ Nộp CV, bảng điểm, research statement cho giáo sư Taehong Kim: taehongkim@cbnu.ac.kr (Deadline: 24/04/2023)
++ Lab info: https://nclab.cbnu.ac.kr
++ Guidelines: https://cia.chungbuk.ac.kr/.../notice/view/wr_id/138/key/180
+Cảm ơn mọi người đã dành thời gian đọc tin 💖💖💖
+=====================================
+Network Computing Laboratory (NCLab) at CBNU is recruiting highly motivated PhD, MS-PhD Integrated, and MS students.
+Requirements:
+👉 A strong academic and research background in computer science, information technology, or a closely related discipline.
+👉Keen research interests in one or more of the following areas: Edge Computing, Container Orchestration and Kubernetes, Machine Learning, Federated Learning, and Edge AI.
+👉Good Python and Java programming abilities, as well as a firm grasp of Linux systems.
+👉Experience in using tools like Git, GitHub, and open-source projects related to the research interests.
+👉Must be able to independently and collaboratively propose, demonstrate, and evaluate new ideas.
+Salary:
+👉Master: 1,400,000 KRW/month
+👉Ph.D: 1,800,000 KRW/month (for first 2 years), 2,000,000 KRW/month (from 3rd year)
+👉Combined: 1,600,000 KRW/month (for first 2 years), same as Ph.D (from 3rd year)
+👉Aside from the basic salary, incentives will be given based on achievement and contribution to the lab, as well as any travel expenses for presenting work at an international conference will also be provided.
+Schedule:
+👉Deadline of application submission: 21 April, 2023
+👉Evaluation and interview, if needed: 22 April – 4 May, 2023
+👉Notification of acceptance: 5 May, 2023
+👉Official admission process: 15 – 26 May, 2023
+* The applicants can see the detail guideline and the required application materials at https://cia.chungbuk.ac.kr/.../notice/view/wr_id/138/key/180. How to apply: If you are interested in our lab, please send your resume, transcripts, and a short research statement (about 300 to 500 words in total) to Prof. Taehong Kim (taehongkim@cbnu.ac.kr). For more details, you can visit our homepage at http://nclab.cbnu.ac.kr</t>
   </si>
 </sst>
 </file>
@@ -317,20 +359,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -647,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6E3FAE0-FEA8-534C-A98C-B63B3E9EAC4A}">
-  <dimension ref="B3:H17"/>
+  <dimension ref="B3:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="68" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,10 +740,10 @@
         <v>8</v>
       </c>
       <c r="E4" s="10"/>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="11"/>
       <c r="H4" s="10" t="s">
         <v>6</v>
       </c>
@@ -714,7 +756,7 @@
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="9"/>
+      <c r="G5" s="11"/>
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
@@ -725,7 +767,7 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="11"/>
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
@@ -736,7 +778,7 @@
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="11"/>
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
@@ -747,7 +789,7 @@
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="11"/>
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
@@ -758,7 +800,7 @@
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
@@ -769,7 +811,7 @@
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="9"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
@@ -780,7 +822,7 @@
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="9"/>
+      <c r="G11" s="11"/>
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
@@ -791,7 +833,7 @@
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="2:8" ht="264" customHeight="1" x14ac:dyDescent="0.2">
@@ -804,13 +846,13 @@
       <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="11" t="s">
         <v>19</v>
       </c>
       <c r="H13" s="10" t="s">
@@ -823,9 +865,9 @@
       <c r="D14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="2:8" ht="264" customHeight="1" x14ac:dyDescent="0.2">
@@ -834,9 +876,9 @@
       <c r="D15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="2:8" ht="409.6" x14ac:dyDescent="0.2">
@@ -866,7 +908,7 @@
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="9" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="6" t="s">
@@ -882,8 +924,75 @@
         <v>35</v>
       </c>
     </row>
+    <row r="18" spans="2:8" ht="185" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="10">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="2:8" ht="185" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="2:8" ht="185" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="2:8" ht="185" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="2:8" ht="185" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="19">
+    <mergeCell ref="F18:F23"/>
+    <mergeCell ref="G18:G23"/>
+    <mergeCell ref="H18:H23"/>
+    <mergeCell ref="E18:E23"/>
+    <mergeCell ref="D18:D23"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C18:C23"/>
     <mergeCell ref="H4:H12"/>
     <mergeCell ref="H13:H15"/>
     <mergeCell ref="G13:G15"/>

</xml_diff>